<commit_message>
v2.1 install new type validation
</commit_message>
<xml_diff>
--- a/userlist/users.xlsx
+++ b/userlist/users.xlsx
@@ -539,17 +539,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>fsdfsd</t>
+          <t>fds</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>432</t>
+          <t>435</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>gfdsfsd</t>
+          <t>432432</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -559,12 +559,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Подключиться к пулу со скидкой ✅</t>
+          <t>Хочу купить оборудование 🔥</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>USD $</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -574,32 +574,32 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>4343</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>43</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>43</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>/password</t>
+          <t>43</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>да</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2023-06-12 23:36:23.261064</t>
+          <t>2023-06-13 10:54:32.282695</t>
         </is>
       </c>
     </row>

</xml_diff>